<commit_message>
added fixe to script
</commit_message>
<xml_diff>
--- a/Python ETL/BASE_DADOS1.9.xlsx
+++ b/Python ETL/BASE_DADOS1.9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolineamarante/Documents/gerenciamento-de-salas-V0.1/Python ETL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Documents\GitHub\gerenciamento-de-salas-V0.1\Python ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D261983-0DEB-D440-8AD6-21F7E80D6E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AA5D04-E984-47A5-8BA9-E7F5D510D3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" activeTab="6" xr2:uid="{DE615C08-F97B-4A36-9702-3D0A64471026}"/>
+    <workbookView xWindow="240" yWindow="2040" windowWidth="28800" windowHeight="11505" xr2:uid="{DE615C08-F97B-4A36-9702-3D0A64471026}"/>
   </bookViews>
   <sheets>
     <sheet name="1_SEMESTRE" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -570,11 +575,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="00000"/>
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1448,7 +1453,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="151">
@@ -1456,7 +1461,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1510,16 +1515,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1543,7 +1548,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1589,7 +1594,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1664,7 +1669,7 @@
     <xf numFmtId="1" fontId="0" fillId="10" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1722,10 +1727,10 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1752,7 +1757,7 @@
     <xf numFmtId="1" fontId="0" fillId="12" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1788,7 +1793,7 @@
     <xf numFmtId="1" fontId="0" fillId="12" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1824,13 +1829,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1845,6 +1850,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1863,18 +1880,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1901,16 +1906,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="50">
     <dxf>
       <font>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
+      <numFmt numFmtId="166" formatCode="h:mm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1993,7 +1998,7 @@
       <font>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="166" formatCode="h:mm;@"/>
+      <numFmt numFmtId="165" formatCode="h:mm;@"/>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
@@ -2433,7 +2438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2731,27 +2736,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCDD7F4-5CE8-447B-8352-1E8B6ACD69B6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="12"/>
-    <col min="5" max="5" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" style="12"/>
-    <col min="7" max="7" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" style="12"/>
-    <col min="9" max="9" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" style="12"/>
-    <col min="11" max="11" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="21.1640625" style="12"/>
+    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="12"/>
+    <col min="5" max="5" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="12"/>
+    <col min="7" max="7" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="12"/>
+    <col min="9" max="9" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="12"/>
+    <col min="11" max="11" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="21.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22">
+    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -2765,18 +2770,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="E1" s="141" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>2</v>
@@ -2815,11 +2820,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="51">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -2858,9 +2863,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>13</v>
@@ -2897,11 +2902,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -2940,9 +2945,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
@@ -2979,27 +2984,27 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="34">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -3038,9 +3043,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
@@ -3077,11 +3082,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="51">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -3120,9 +3125,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
@@ -3159,11 +3164,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="51">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -3202,9 +3207,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
@@ -3241,21 +3246,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="14" customHeight="1"/>
+    <row r="15" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3305,22 +3310,22 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="32" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="32" customWidth="1"/>
     <col min="4" max="4" width="17" style="32"/>
-    <col min="5" max="5" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="32"/>
-    <col min="7" max="7" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="32"/>
-    <col min="9" max="9" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="32"/>
-    <col min="11" max="11" width="7.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="17" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="44">
+    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -3334,18 +3339,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>1</v>
@@ -3384,11 +3389,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="34">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -3427,9 +3432,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>1</v>
@@ -3466,11 +3471,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -3509,9 +3514,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
@@ -3548,27 +3553,27 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="34">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -3607,9 +3612,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
@@ -3646,11 +3651,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="34">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -3689,9 +3694,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
@@ -3728,11 +3733,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="34">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -3771,9 +3776,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
@@ -3867,15 +3872,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="32" customWidth="1"/>
-    <col min="3" max="3" width="7.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="18.1640625" style="32"/>
+    <col min="1" max="1" width="8.28515625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="18.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22">
+    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -3889,18 +3894,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>1</v>
@@ -3939,11 +3944,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="34">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -3982,9 +3987,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
@@ -4021,11 +4026,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -4064,9 +4069,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>1</v>
@@ -4103,27 +4108,27 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -4162,9 +4167,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
@@ -4201,11 +4206,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="43.5" customHeight="1">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -4244,9 +4249,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>1</v>
@@ -4283,11 +4288,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="48" customHeight="1">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -4326,9 +4331,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17" thickBot="1">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>1</v>
@@ -4367,18 +4372,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4434,9 +4439,9 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="22">
+    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4450,18 +4455,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>2</v>
@@ -4500,11 +4505,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="68">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -4543,9 +4548,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>9</v>
@@ -4582,11 +4587,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="68">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -4625,9 +4630,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>9</v>
@@ -4664,27 +4669,27 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="51">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -4723,9 +4728,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>1</v>
@@ -4762,11 +4767,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="68">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -4805,9 +4810,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
@@ -4844,11 +4849,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="68">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -4887,9 +4892,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
@@ -4928,18 +4933,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4984,13 +4989,13 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="35.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="16" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21.75" customHeight="1">
+    <row r="1" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -5004,18 +5009,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="35.25" customHeight="1">
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>2</v>
@@ -5054,11 +5059,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -5097,9 +5102,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
@@ -5136,11 +5141,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -5179,9 +5184,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
@@ -5218,27 +5223,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -5277,9 +5282,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
@@ -5316,11 +5321,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -5359,9 +5364,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
@@ -5398,11 +5403,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -5441,9 +5446,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="35.25" customHeight="1">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
@@ -5482,18 +5487,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5537,13 +5542,13 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="14.6640625" style="32"/>
+    <col min="1" max="1" width="8.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="14.7109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" customHeight="1">
+    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -5557,18 +5562,18 @@
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="141" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="142"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <f>VLOOKUP(B2,Tabela4[#All],2,FALSE)</f>
         <v>2</v>
@@ -5607,11 +5612,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="34">
-      <c r="A3" s="139" t="s">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="140">
+      <c r="B3" s="134">
         <v>0.78125</v>
       </c>
       <c r="C3" s="2">
@@ -5650,9 +5655,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32">
-      <c r="A4" s="139"/>
-      <c r="B4" s="140"/>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
@@ -5689,11 +5694,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="51">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="140">
+      <c r="B5" s="134">
         <v>0.81597222222222221</v>
       </c>
       <c r="C5" s="2">
@@ -5732,9 +5737,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="32">
-      <c r="A6" s="139"/>
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
@@ -5771,27 +5776,27 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="136"/>
-    </row>
-    <row r="8" spans="1:12" ht="51">
-      <c r="A8" s="139" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="140">
+      <c r="B8" s="134">
         <v>0.85763888888888884</v>
       </c>
       <c r="C8" s="2">
@@ -5830,9 +5835,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="32">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
@@ -5869,11 +5874,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="51">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="140">
+      <c r="B10" s="134">
         <v>0.89236111111111116</v>
       </c>
       <c r="C10" s="2">
@@ -5912,9 +5917,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="32">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
@@ -5951,11 +5956,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="51">
-      <c r="A12" s="139" t="s">
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="140">
+      <c r="B12" s="134">
         <v>0.92708333333333337</v>
       </c>
       <c r="C12" s="2">
@@ -5994,9 +5999,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="32">
-      <c r="A13" s="141"/>
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
@@ -6035,18 +6040,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6092,36 +6097,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF6508E-B8F4-43C4-AACB-99409B526617}">
   <dimension ref="B1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="39"/>
-    <col min="4" max="4" width="2.5" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" style="73" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.83203125" customWidth="1"/>
-    <col min="11" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.5" customWidth="1"/>
-    <col min="16" max="16" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.83203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5" customWidth="1"/>
-    <col min="19" max="19" width="15.5" customWidth="1"/>
-    <col min="20" max="20" width="15.5" style="39" customWidth="1"/>
-    <col min="16384" max="16384" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="39"/>
+    <col min="4" max="4" width="2.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.42578125" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="39" customWidth="1"/>
+    <col min="16384" max="16384" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:20" ht="35.5" customHeight="1">
+    <row r="1" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:20" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="146" t="s">
         <v>73</v>
       </c>
@@ -6149,7 +6154,7 @@
       </c>
       <c r="T2" s="147"/>
     </row>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
         <v>78</v>
       </c>
@@ -6199,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="74" t="s">
         <v>121</v>
       </c>
@@ -6251,7 +6256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>24</v>
       </c>
@@ -6303,7 +6308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
         <v>6</v>
       </c>
@@ -6355,7 +6360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
         <v>4</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="16" thickBot="1">
+    <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="34" t="s">
         <v>48</v>
       </c>
@@ -6459,7 +6464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="16" thickBot="1">
+    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="34" t="s">
         <v>34</v>
       </c>
@@ -6505,7 +6510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
         <v>29</v>
       </c>
@@ -6546,7 +6551,7 @@
       <c r="O10" s="12"/>
       <c r="Q10" s="15"/>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>30</v>
       </c>
@@ -6587,7 +6592,7 @@
       <c r="O11" s="12"/>
       <c r="Q11" s="15"/>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
         <v>43</v>
       </c>
@@ -6628,7 +6633,7 @@
       <c r="O12" s="12"/>
       <c r="Q12" s="15"/>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
         <v>47</v>
       </c>
@@ -6669,7 +6674,7 @@
       <c r="O13" s="12"/>
       <c r="Q13" s="15"/>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="34" t="s">
         <v>31</v>
       </c>
@@ -6710,7 +6715,7 @@
       <c r="O14" s="12"/>
       <c r="Q14" s="15"/>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
         <v>38</v>
       </c>
@@ -6751,7 +6756,7 @@
       <c r="O15" s="12"/>
       <c r="Q15" s="15"/>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>49</v>
       </c>
@@ -6792,7 +6797,7 @@
       <c r="O16" s="12"/>
       <c r="Q16" s="15"/>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="34" t="s">
         <v>40</v>
       </c>
@@ -6833,7 +6838,7 @@
       <c r="O17" s="12"/>
       <c r="Q17" s="15"/>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
@@ -6874,7 +6879,7 @@
       <c r="O18" s="12"/>
       <c r="Q18" s="15"/>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
         <v>21</v>
       </c>
@@ -6915,7 +6920,7 @@
       <c r="O19" s="12"/>
       <c r="Q19" s="15"/>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
         <v>33</v>
       </c>
@@ -6956,7 +6961,7 @@
       <c r="O20" s="12"/>
       <c r="Q20" s="15"/>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="34" t="s">
         <v>39</v>
       </c>
@@ -6997,7 +7002,7 @@
       <c r="O21" s="12"/>
       <c r="Q21" s="15"/>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
         <v>53</v>
       </c>
@@ -7038,7 +7043,7 @@
       <c r="O22" s="12"/>
       <c r="Q22" s="15"/>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>44</v>
       </c>
@@ -7079,7 +7084,7 @@
       <c r="O23" s="12"/>
       <c r="Q23" s="15"/>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="34" t="s">
         <v>25</v>
       </c>
@@ -7107,7 +7112,7 @@
       <c r="O24" s="12"/>
       <c r="Q24" s="15"/>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="34" t="s">
         <v>32</v>
       </c>
@@ -7135,7 +7140,7 @@
       <c r="O25" s="12"/>
       <c r="Q25" s="15"/>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="34" t="s">
         <v>23</v>
       </c>
@@ -7163,7 +7168,7 @@
       <c r="O26" s="12"/>
       <c r="Q26" s="15"/>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="34" t="s">
         <v>52</v>
       </c>
@@ -7191,7 +7196,7 @@
       <c r="O27" s="12"/>
       <c r="Q27" s="15"/>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="34" t="s">
         <v>22</v>
       </c>
@@ -7219,7 +7224,7 @@
       <c r="O28" s="12"/>
       <c r="Q28" s="15"/>
     </row>
-    <row r="29" spans="2:17">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
         <v>50</v>
       </c>
@@ -7247,7 +7252,7 @@
       <c r="O29" s="12"/>
       <c r="Q29" s="15"/>
     </row>
-    <row r="30" spans="2:17">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="34" t="s">
         <v>28</v>
       </c>
@@ -7275,7 +7280,7 @@
       <c r="O30" s="12"/>
       <c r="Q30" s="15"/>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
         <v>41</v>
       </c>
@@ -7295,7 +7300,7 @@
       <c r="O31" s="12"/>
       <c r="Q31" s="15"/>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="34" t="s">
         <v>51</v>
       </c>
@@ -7315,7 +7320,7 @@
       <c r="O32" s="12"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="34" t="s">
         <v>42</v>
       </c>
@@ -7331,7 +7336,7 @@
       <c r="M33" s="15"/>
       <c r="N33" s="17"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="34" t="s">
         <v>56</v>
       </c>
@@ -7347,7 +7352,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="17"/>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="34" t="s">
         <v>62</v>
       </c>
@@ -7363,7 +7368,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="17"/>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
         <v>70</v>
       </c>
@@ -7379,7 +7384,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
         <v>58</v>
       </c>
@@ -7395,7 +7400,7 @@
       <c r="M37" s="15"/>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="34" t="s">
         <v>59</v>
       </c>
@@ -7411,7 +7416,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="17"/>
     </row>
-    <row r="39" spans="2:14" ht="15" customHeight="1">
+    <row r="39" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="34" t="s">
         <v>57</v>
       </c>
@@ -7427,7 +7432,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="2:14" ht="15" customHeight="1">
+    <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="34" t="s">
         <v>60</v>
       </c>
@@ -7443,7 +7448,7 @@
       <c r="M40" s="15"/>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="2:14" ht="15" customHeight="1">
+    <row r="41" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="34" t="s">
         <v>61</v>
       </c>
@@ -7459,7 +7464,7 @@
       <c r="M41" s="15"/>
       <c r="N41" s="17"/>
     </row>
-    <row r="42" spans="2:14" ht="15" customHeight="1">
+    <row r="42" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="34" t="s">
         <v>65</v>
       </c>
@@ -7475,7 +7480,7 @@
       <c r="M42" s="15"/>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="2:14" ht="15" customHeight="1">
+    <row r="43" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="34" t="s">
         <v>71</v>
       </c>
@@ -7491,7 +7496,7 @@
       <c r="M43" s="15"/>
       <c r="N43" s="17"/>
     </row>
-    <row r="44" spans="2:14" ht="15" customHeight="1">
+    <row r="44" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="34" t="s">
         <v>66</v>
       </c>
@@ -7507,7 +7512,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="17"/>
     </row>
-    <row r="45" spans="2:14" ht="15" customHeight="1">
+    <row r="45" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="34" t="s">
         <v>68</v>
       </c>
@@ -7523,7 +7528,7 @@
       <c r="M45" s="15"/>
       <c r="N45" s="17"/>
     </row>
-    <row r="46" spans="2:14" ht="15" customHeight="1">
+    <row r="46" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="34" t="s">
         <v>72</v>
       </c>
@@ -7539,7 +7544,7 @@
       <c r="M46" s="15"/>
       <c r="N46" s="17"/>
     </row>
-    <row r="47" spans="2:14" ht="15" customHeight="1">
+    <row r="47" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="34" t="s">
         <v>67</v>
       </c>
@@ -7555,7 +7560,7 @@
       <c r="M47" s="15"/>
       <c r="N47" s="17"/>
     </row>
-    <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
+    <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="36" t="s">
         <v>69</v>
       </c>
@@ -7608,23 +7613,23 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
     <col min="2" max="2" width="5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="72" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="12"/>
+    <col min="8" max="8" width="12.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26">
+    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B1" s="148" t="s">
         <v>168</v>
       </c>
@@ -7638,7 +7643,7 @@
       <c r="J1" s="149"/>
       <c r="K1" s="150"/>
     </row>
-    <row r="2" spans="1:11" ht="16" thickBot="1">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>106</v>
       </c>
@@ -7673,7 +7678,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="100" t="s">
         <v>115</v>
       </c>
@@ -7712,7 +7717,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>117</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="110" t="s">
         <v>118</v>
       </c>
@@ -7790,7 +7795,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="109" t="s">
         <v>119</v>
       </c>
@@ -7829,7 +7834,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="110" t="s">
         <v>120</v>
       </c>
@@ -7869,7 +7874,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="109" t="s">
         <v>115</v>
       </c>
@@ -7909,7 +7914,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="110" t="s">
         <v>117</v>
       </c>
@@ -7949,7 +7954,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="109" t="s">
         <v>118</v>
       </c>
@@ -7989,7 +7994,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="110" t="s">
         <v>119</v>
       </c>
@@ -8029,7 +8034,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="109" t="s">
         <v>120</v>
       </c>
@@ -8069,7 +8074,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="110" t="s">
         <v>115</v>
       </c>
@@ -8109,7 +8114,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="109" t="s">
         <v>117</v>
       </c>
@@ -8149,7 +8154,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="110" t="s">
         <v>118</v>
       </c>
@@ -8189,7 +8194,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="109" t="s">
         <v>119</v>
       </c>
@@ -8229,7 +8234,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="110" t="s">
         <v>120</v>
       </c>
@@ -8269,7 +8274,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="109" t="s">
         <v>115</v>
       </c>
@@ -8309,7 +8314,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="110" t="s">
         <v>117</v>
       </c>
@@ -8349,7 +8354,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="109" t="s">
         <v>118</v>
       </c>
@@ -8389,7 +8394,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="110" t="s">
         <v>119</v>
       </c>
@@ -8429,7 +8434,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="109" t="s">
         <v>120</v>
       </c>
@@ -8469,7 +8474,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="110" t="s">
         <v>115</v>
       </c>
@@ -8509,7 +8514,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="109" t="s">
         <v>117</v>
       </c>
@@ -8549,7 +8554,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="111" t="s">
         <v>118</v>
       </c>
@@ -8589,7 +8594,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="109" t="s">
         <v>119</v>
       </c>
@@ -8629,7 +8634,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16" thickBot="1">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="112" t="s">
         <v>120</v>
       </c>
@@ -8669,7 +8674,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="100" t="s">
         <v>115</v>
       </c>
@@ -8709,7 +8714,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="109" t="s">
         <v>117</v>
       </c>
@@ -8748,7 +8753,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="110" t="s">
         <v>118</v>
       </c>
@@ -8787,7 +8792,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="109" t="s">
         <v>119</v>
       </c>
@@ -8826,7 +8831,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="110" t="s">
         <v>120</v>
       </c>
@@ -8865,7 +8870,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="109" t="s">
         <v>115</v>
       </c>
@@ -8904,7 +8909,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="110" t="s">
         <v>117</v>
       </c>
@@ -8943,7 +8948,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="109" t="s">
         <v>118</v>
       </c>
@@ -8982,7 +8987,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="110" t="s">
         <v>119</v>
       </c>
@@ -9021,7 +9026,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="109" t="s">
         <v>120</v>
       </c>
@@ -9060,7 +9065,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="110" t="s">
         <v>115</v>
       </c>
@@ -9099,7 +9104,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="109" t="s">
         <v>117</v>
       </c>
@@ -9138,7 +9143,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="110" t="s">
         <v>118</v>
       </c>
@@ -9177,7 +9182,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="109" t="s">
         <v>119</v>
       </c>
@@ -9216,7 +9221,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="110" t="s">
         <v>120</v>
       </c>
@@ -9255,7 +9260,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="109" t="s">
         <v>115</v>
       </c>
@@ -9294,7 +9299,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="110" t="s">
         <v>117</v>
       </c>
@@ -9333,7 +9338,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="109" t="s">
         <v>118</v>
       </c>
@@ -9372,7 +9377,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="110" t="s">
         <v>119</v>
       </c>
@@ -9411,7 +9416,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="109" t="s">
         <v>120</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="110" t="s">
         <v>115</v>
       </c>
@@ -9489,7 +9494,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="109" t="s">
         <v>117</v>
       </c>
@@ -9528,7 +9533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="111" t="s">
         <v>118</v>
       </c>
@@ -9567,7 +9572,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="109" t="s">
         <v>119</v>
       </c>
@@ -9606,7 +9611,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="16" thickBot="1">
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="112" t="s">
         <v>120</v>
       </c>
@@ -9645,7 +9650,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="100" t="s">
         <v>115</v>
       </c>
@@ -9684,7 +9689,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="109" t="s">
         <v>117</v>
       </c>
@@ -9723,7 +9728,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="110" t="s">
         <v>118</v>
       </c>
@@ -9762,7 +9767,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="109" t="s">
         <v>119</v>
       </c>
@@ -9801,7 +9806,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="110" t="s">
         <v>120</v>
       </c>
@@ -9840,7 +9845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="109" t="s">
         <v>115</v>
       </c>
@@ -9879,7 +9884,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="110" t="s">
         <v>117</v>
       </c>
@@ -9918,7 +9923,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="109" t="s">
         <v>118</v>
       </c>
@@ -9957,7 +9962,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="110" t="s">
         <v>119</v>
       </c>
@@ -9996,7 +10001,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="109" t="s">
         <v>120</v>
       </c>
@@ -10035,7 +10040,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="110" t="s">
         <v>115</v>
       </c>
@@ -10074,7 +10079,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="109" t="s">
         <v>117</v>
       </c>
@@ -10113,7 +10118,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="110" t="s">
         <v>118</v>
       </c>
@@ -10152,7 +10157,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="109" t="s">
         <v>119</v>
       </c>
@@ -10191,7 +10196,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="110" t="s">
         <v>120</v>
       </c>
@@ -10230,7 +10235,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="109" t="s">
         <v>115</v>
       </c>
@@ -10269,7 +10274,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="110" t="s">
         <v>117</v>
       </c>
@@ -10307,7 +10312,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="109" t="s">
         <v>118</v>
       </c>
@@ -10345,7 +10350,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="110" t="s">
         <v>119</v>
       </c>
@@ -10383,7 +10388,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="109" t="s">
         <v>120</v>
       </c>
@@ -10421,7 +10426,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="110" t="s">
         <v>115</v>
       </c>
@@ -10460,7 +10465,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="109" t="s">
         <v>117</v>
       </c>
@@ -10499,7 +10504,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="111" t="s">
         <v>118</v>
       </c>
@@ -10538,7 +10543,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="109" t="s">
         <v>119</v>
       </c>
@@ -10577,7 +10582,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="16" thickBot="1">
+    <row r="77" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="112" t="s">
         <v>120</v>
       </c>
@@ -10616,7 +10621,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="100" t="s">
         <v>115</v>
       </c>
@@ -10655,7 +10660,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="109" t="s">
         <v>117</v>
       </c>
@@ -10694,7 +10699,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="110" t="s">
         <v>118</v>
       </c>
@@ -10733,7 +10738,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="109" t="s">
         <v>119</v>
       </c>
@@ -10772,7 +10777,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="110" t="s">
         <v>120</v>
       </c>
@@ -10811,7 +10816,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="109" t="s">
         <v>115</v>
       </c>
@@ -10850,7 +10855,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="110" t="s">
         <v>117</v>
       </c>
@@ -10889,7 +10894,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="109" t="s">
         <v>118</v>
       </c>
@@ -10928,7 +10933,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="110" t="s">
         <v>119</v>
       </c>
@@ -10967,7 +10972,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="109" t="s">
         <v>120</v>
       </c>
@@ -11006,7 +11011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="110" t="s">
         <v>115</v>
       </c>
@@ -11045,7 +11050,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="109" t="s">
         <v>117</v>
       </c>
@@ -11084,7 +11089,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="110" t="s">
         <v>118</v>
       </c>
@@ -11123,7 +11128,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="109" t="s">
         <v>119</v>
       </c>
@@ -11162,7 +11167,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="110" t="s">
         <v>120</v>
       </c>
@@ -11201,7 +11206,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="109" t="s">
         <v>115</v>
       </c>
@@ -11240,7 +11245,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="110" t="s">
         <v>117</v>
       </c>
@@ -11279,7 +11284,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="109" t="s">
         <v>118</v>
       </c>
@@ -11318,7 +11323,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="110" t="s">
         <v>119</v>
       </c>
@@ -11357,7 +11362,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="109" t="s">
         <v>120</v>
       </c>
@@ -11396,7 +11401,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="110" t="s">
         <v>115</v>
       </c>
@@ -11435,7 +11440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="109" t="s">
         <v>117</v>
       </c>
@@ -11474,7 +11479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="111" t="s">
         <v>118</v>
       </c>
@@ -11513,7 +11518,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="109" t="s">
         <v>119</v>
       </c>
@@ -11552,7 +11557,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="16" thickBot="1">
+    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="112" t="s">
         <v>120</v>
       </c>
@@ -11591,7 +11596,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="100" t="s">
         <v>115</v>
       </c>
@@ -11630,7 +11635,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="109" t="s">
         <v>117</v>
       </c>
@@ -11669,7 +11674,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="110" t="s">
         <v>118</v>
       </c>
@@ -11708,7 +11713,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="109" t="s">
         <v>119</v>
       </c>
@@ -11747,7 +11752,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="110" t="s">
         <v>120</v>
       </c>
@@ -11786,7 +11791,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="109" t="s">
         <v>115</v>
       </c>
@@ -11825,7 +11830,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="110" t="s">
         <v>117</v>
       </c>
@@ -11864,7 +11869,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="109" t="s">
         <v>118</v>
       </c>
@@ -11903,7 +11908,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="110" t="s">
         <v>119</v>
       </c>
@@ -11942,7 +11947,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="109" t="s">
         <v>120</v>
       </c>
@@ -11981,7 +11986,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="110" t="s">
         <v>115</v>
       </c>
@@ -12020,7 +12025,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="109" t="s">
         <v>117</v>
       </c>
@@ -12059,7 +12064,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="110" t="s">
         <v>118</v>
       </c>
@@ -12098,7 +12103,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="109" t="s">
         <v>119</v>
       </c>
@@ -12137,7 +12142,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="110" t="s">
         <v>120</v>
       </c>
@@ -12176,7 +12181,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="109" t="s">
         <v>115</v>
       </c>
@@ -12215,7 +12220,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="110" t="s">
         <v>117</v>
       </c>
@@ -12254,7 +12259,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="109" t="s">
         <v>118</v>
       </c>
@@ -12293,7 +12298,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="110" t="s">
         <v>119</v>
       </c>
@@ -12332,7 +12337,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="109" t="s">
         <v>120</v>
       </c>
@@ -12371,7 +12376,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="110" t="s">
         <v>115</v>
       </c>
@@ -12410,7 +12415,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="109" t="s">
         <v>117</v>
       </c>
@@ -12449,7 +12454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="111" t="s">
         <v>118</v>
       </c>
@@ -12488,7 +12493,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="109" t="s">
         <v>119</v>
       </c>
@@ -12527,7 +12532,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="16" thickBot="1">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="112" t="s">
         <v>120</v>
       </c>
@@ -12566,7 +12571,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="95" t="s">
         <v>115</v>
       </c>
@@ -12605,7 +12610,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="58" t="s">
         <v>117</v>
       </c>
@@ -12644,7 +12649,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="59" t="s">
         <v>118</v>
       </c>
@@ -12683,7 +12688,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="58" t="s">
         <v>119</v>
       </c>
@@ -12722,7 +12727,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="59" t="s">
         <v>120</v>
       </c>
@@ -12761,7 +12766,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="58" t="s">
         <v>115</v>
       </c>
@@ -12800,7 +12805,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="59" t="s">
         <v>117</v>
       </c>
@@ -12839,7 +12844,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="58" t="s">
         <v>118</v>
       </c>
@@ -12878,7 +12883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="59" t="s">
         <v>119</v>
       </c>
@@ -12917,7 +12922,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="58" t="s">
         <v>120</v>
       </c>
@@ -12956,7 +12961,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="59" t="s">
         <v>115</v>
       </c>
@@ -12995,7 +13000,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="58" t="s">
         <v>117</v>
       </c>
@@ -13034,7 +13039,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="59" t="s">
         <v>118</v>
       </c>
@@ -13073,7 +13078,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="58" t="s">
         <v>119</v>
       </c>
@@ -13112,7 +13117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="59" t="s">
         <v>120</v>
       </c>
@@ -13151,7 +13156,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="58" t="s">
         <v>115</v>
       </c>
@@ -13190,7 +13195,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="59" t="s">
         <v>117</v>
       </c>
@@ -13229,7 +13234,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="58" t="s">
         <v>118</v>
       </c>
@@ -13268,7 +13273,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="59" t="s">
         <v>119</v>
       </c>
@@ -13307,7 +13312,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="58" t="s">
         <v>120</v>
       </c>
@@ -13346,7 +13351,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="59" t="s">
         <v>115</v>
       </c>
@@ -13385,7 +13390,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="58" t="s">
         <v>117</v>
       </c>
@@ -13424,7 +13429,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="60" t="s">
         <v>118</v>
       </c>
@@ -13463,7 +13468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="58" t="s">
         <v>119</v>
       </c>
@@ -13502,7 +13507,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="16" thickBot="1">
+    <row r="152" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="61" t="s">
         <v>120</v>
       </c>
@@ -13559,6 +13564,23 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8b482999-19eb-4912-ba0e-318ec40975bd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E158B1B397417E47B82773C62AE92C77" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7b926754ab08cd6eb658e66ec26ff8a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8b482999-19eb-4912-ba0e-318ec40975bd" xmlns:ns4="cdcb5d5f-3806-4c84-af96-b897b3155cb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c26c19dbdbb4d4cab911bad2087a66f" ns3:_="" ns4:_="">
     <xsd:import namespace="8b482999-19eb-4912-ba0e-318ec40975bd"/>
@@ -13793,23 +13815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8b482999-19eb-4912-ba0e-318ec40975bd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0479E3B0-EA41-4C73-89CE-318EC5E54B4A}">
   <ds:schemaRefs>
@@ -13819,6 +13824,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08DBE0B6-649A-42A6-AA7A-69D2466B3D18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8b482999-19eb-4912-ba0e-318ec40975bd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{513CCFD7-6341-4F0F-AF01-C552F653B738}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3C15EC-2DF5-465A-BE5C-C4D427022D39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13835,22 +13858,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{513CCFD7-6341-4F0F-AF01-C552F653B738}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08DBE0B6-649A-42A6-AA7A-69D2466B3D18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8b482999-19eb-4912-ba0e-318ec40975bd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>